<commit_message>
Lectura y Validación de Movimientos del XML generando Objetos tipo Movimiento
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>NroContrato</t>
   </si>
@@ -30,12 +30,6 @@
   </si>
   <si>
     <t>PRODUCTOR</t>
-  </si>
-  <si>
-    <t>111111111111</t>
-  </si>
-  <si>
-    <t>Prueba 1</t>
   </si>
   <si>
     <t>ILDEFONSO MUÑECAS 167 - B° CENTRO</t>
@@ -225,23 +219,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s" s="2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" t="s" s="2">
         <v>6</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>8</v>
       </c>
       <c r="E2" t="n" s="2">
         <v>4000.0</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -249,19 +237,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="2">
         <v>10</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>12</v>
       </c>
       <c r="E3" t="n" s="2">
         <v>4427.0</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -269,19 +257,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="2">
         <v>13</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>15</v>
       </c>
       <c r="E4" t="n" s="2">
         <v>7000.0</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -289,19 +277,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s" s="2">
         <v>17</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>19</v>
       </c>
       <c r="E5" t="n" s="2">
         <v>8000.0</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
@@ -309,19 +297,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s" s="2">
         <v>21</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>23</v>
       </c>
       <c r="E6" t="n" s="2">
         <v>7600.0</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -329,19 +317,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s" s="2">
         <v>24</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>26</v>
       </c>
       <c r="E7" t="n" s="2">
         <v>1036.0</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -349,19 +337,19 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s" s="2">
         <v>28</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>30</v>
       </c>
       <c r="E8" t="n" s="2">
         <v>1002.0</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -369,19 +357,19 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s" s="2">
         <v>31</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>33</v>
       </c>
       <c r="E9" t="n" s="2">
         <v>1872.0</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
@@ -389,19 +377,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s" s="2">
         <v>35</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>37</v>
       </c>
       <c r="E10" t="n" s="2">
         <v>1437.0</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -409,19 +397,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s" s="2">
         <v>38</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>40</v>
       </c>
       <c r="E11" t="n" s="2">
         <v>1822.0</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generación del Excel con dos solapas
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Empresas" r:id="rId3" sheetId="1"/>
+    <sheet name="Movimientos" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>NroContrato</t>
   </si>
@@ -32,6 +33,12 @@
     <t>PRODUCTOR</t>
   </si>
   <si>
+    <t>111111111111</t>
+  </si>
+  <si>
+    <t>Prueba 1</t>
+  </si>
+  <si>
     <t>ILDEFONSO MUÑECAS 167 - B° CENTRO</t>
   </si>
   <si>
@@ -129,6 +136,21 @@
   </si>
   <si>
     <t>REPUBLICA ARGENTINA 2029 - B° VILLA SPINOLA</t>
+  </si>
+  <si>
+    <t>SaldoCtaCte</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>Importe</t>
+  </si>
+  <si>
+    <t>Pago</t>
+  </si>
+  <si>
+    <t>Debito</t>
   </si>
 </sst>
 </file>
@@ -136,13 +158,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -174,10 +205,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -219,17 +252,23 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>7</v>
+      </c>
       <c r="D2" t="s" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n" s="2">
         <v>4000.0</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -237,19 +276,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" t="n" s="2">
         <v>4427.0</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -257,19 +296,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4" t="n" s="2">
         <v>7000.0</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -277,19 +316,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" t="n" s="2">
         <v>8000.0</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -297,19 +336,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" t="n" s="2">
         <v>7600.0</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -317,19 +356,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" t="n" s="2">
         <v>1036.0</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
@@ -337,19 +376,19 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E8" t="n" s="2">
         <v>1002.0</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
@@ -357,19 +396,19 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E9" t="n" s="2">
         <v>1872.0</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
@@ -377,19 +416,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E10" t="n" s="2">
         <v>1437.0</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
@@ -397,19 +436,206 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" t="n" s="2">
         <v>1822.0</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="18.2890625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="17.6484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.1640625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.28515625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="3">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="3">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n" s="4">
+        <v>-21802.12</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D2" t="n" s="4">
+        <v>21802.19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n" s="4">
+        <v>-46791.12</v>
+      </c>
+      <c r="C3" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D3" t="n" s="4">
+        <v>46739.28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n" s="4">
+        <v>-25665.9</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D4" t="n" s="4">
+        <v>25665.97</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="n" s="4">
+        <v>-12410.67</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D5" t="n" s="4">
+        <v>12305.41</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="n" s="4">
+        <v>1663.86</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D6" t="n" s="4">
+        <v>2395.25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="B7" t="n" s="4">
+        <v>-731.39</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>45</v>
+      </c>
+      <c r="D7" t="n" s="4">
+        <v>740.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="B8" t="n" s="4">
+        <v>-45268.6</v>
+      </c>
+      <c r="C8" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D8" t="n" s="4">
+        <v>45268.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="B9" t="n" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="C9" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D9" t="n" s="4">
+        <v>3835.96</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="B10" t="n" s="4">
+        <v>-2854.09</v>
+      </c>
+      <c r="C10" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D10" t="n" s="4">
+        <v>3105.25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="B11" t="n" s="4">
+        <v>-414.46</v>
+      </c>
+      <c r="C11" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D11" t="n" s="4">
+        <v>573.23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="B12" t="n" s="4">
+        <v>-182510.4</v>
+      </c>
+      <c r="C12" t="s" s="4">
+        <v>44</v>
+      </c>
+      <c r="D12" t="n" s="4">
+        <v>184528.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>